<commit_message>
partially fixed form submission
</commit_message>
<xml_diff>
--- a/Extracted_Data.xlsx
+++ b/Extracted_Data.xlsx
@@ -9,12 +9,18 @@
     <sheet name="chrome_Results_20250829_114222" r:id="rId3" sheetId="1"/>
     <sheet name="chrome_Results_20250829_114340" r:id="rId4" sheetId="2"/>
     <sheet name="edge_Results_20250829_114340" r:id="rId5" sheetId="3"/>
+    <sheet name="chrome_Results_20250830_160934" r:id="rId6" sheetId="4"/>
+    <sheet name="chrome_Results_20250830_161516" r:id="rId7" sheetId="5"/>
+    <sheet name="edge_Results_20250830_162148" r:id="rId8" sheetId="6"/>
+    <sheet name="chrome_Results_20250830_162154" r:id="rId9" sheetId="7"/>
+    <sheet name="edge_Results_20250830_162607" r:id="rId10" sheetId="8"/>
+    <sheet name="chrome_Results_20250830_162626" r:id="rId11" sheetId="9"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="53">
   <si>
     <t>Language</t>
   </si>
@@ -180,13 +186,43 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="10">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -224,11 +260,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -1035,4 +1077,1612 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:B48"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="4">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="0">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="0">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="0">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="0">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="0">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="0">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="0">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="0">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="0">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s" s="0">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s" s="0">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s" s="0">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s" s="0">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s" s="0">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="0">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s" s="0">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s" s="0">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s" s="0">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s" s="0">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s" s="0">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s" s="0">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="0">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="0">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="0">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="0">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="0">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:B48"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="5">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="0">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="0">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="0">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="0">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="0">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="0">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="0">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="0">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="0">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s" s="0">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s" s="0">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s" s="0">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s" s="0">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s" s="0">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="0">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s" s="0">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s" s="0">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s" s="0">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s" s="0">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s" s="0">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s" s="0">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="0">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="0">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="0">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="0">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="0">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:B48"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="6">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="0">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="0">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="0">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="0">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="0">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="0">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="0">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="0">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="0">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s" s="0">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s" s="0">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s" s="0">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s" s="0">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s" s="0">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="0">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s" s="0">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s" s="0">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s" s="0">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s" s="0">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s" s="0">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s" s="0">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="0">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="0">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="0">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="0">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="0">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:B48"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="7">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="0">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="0">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="0">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="0">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="0">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="0">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="0">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="0">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="0">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s" s="0">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s" s="0">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s" s="0">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s" s="0">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s" s="0">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="0">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s" s="0">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s" s="0">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s" s="0">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s" s="0">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s" s="0">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s" s="0">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="0">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="0">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="0">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="0">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="0">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:B48"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="8">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="0">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="0">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="0">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="0">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="0">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="0">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="0">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="0">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="0">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s" s="0">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s" s="0">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s" s="0">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s" s="0">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s" s="0">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="0">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s" s="0">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s" s="0">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s" s="0">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s" s="0">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s" s="0">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s" s="0">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="0">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="0">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="0">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="0">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="0">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:B48"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="9">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="0">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="0">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="0">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="0">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="0">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="0">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="0">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="0">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="0">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s" s="0">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s" s="0">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s" s="0">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s" s="0">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s" s="0">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="0">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s" s="0">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s" s="0">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s" s="0">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s" s="0">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s" s="0">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s" s="0">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="0">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="0">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="0">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="0">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="0">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat:added execute condition to test data
fixes:ExcelReader to read the execute colum
</commit_message>
<xml_diff>
--- a/Extracted_Data.xlsx
+++ b/Extracted_Data.xlsx
@@ -6,24 +6,24 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="chrome_Results_20250829_114222" r:id="rId3" sheetId="1"/>
-    <sheet name="chrome_Results_20250829_114340" r:id="rId4" sheetId="2"/>
-    <sheet name="edge_Results_20250829_114340" r:id="rId5" sheetId="3"/>
-    <sheet name="chrome_Results_20250830_160934" r:id="rId6" sheetId="4"/>
-    <sheet name="chrome_Results_20250830_161516" r:id="rId7" sheetId="5"/>
-    <sheet name="edge_Results_20250830_162148" r:id="rId8" sheetId="6"/>
-    <sheet name="chrome_Results_20250830_162154" r:id="rId9" sheetId="7"/>
-    <sheet name="edge_Results_20250830_162607" r:id="rId10" sheetId="8"/>
-    <sheet name="chrome_Results_20250830_162626" r:id="rId11" sheetId="9"/>
-    <sheet name="edge_Results_20250901_154242" r:id="rId12" sheetId="10"/>
-    <sheet name="chrome_Results_20250901_154244" r:id="rId13" sheetId="11"/>
-    <sheet name="edge_CourseDetails_20250901_154" r:id="rId14" sheetId="12"/>
+    <sheet name="edge_Results_20250903_094411" r:id="rId3" sheetId="1"/>
+    <sheet name="chrome_Results_20250903_094415" r:id="rId4" sheetId="2"/>
+    <sheet name="edge_CourseDetails_20250903_094" r:id="rId5" sheetId="3"/>
+    <sheet name="chrome_CourseDetails_20250903_0" r:id="rId6" sheetId="4"/>
+    <sheet name="edge_Results_20250903_100017" r:id="rId7" sheetId="5"/>
+    <sheet name="chrome_Results_20250903_100034" r:id="rId8" sheetId="6"/>
+    <sheet name="edge_CourseDetails_20250903_100" r:id="rId9" sheetId="7"/>
+    <sheet name="chrome_CourseDetails_20250903_1" r:id="rId10" sheetId="8"/>
+    <sheet name="chrome_Results_20250903_100355" r:id="rId11" sheetId="9"/>
+    <sheet name="edge_Results_20250903_100409" r:id="rId12" sheetId="10"/>
+    <sheet name="edge_Results_20250903_100724" r:id="rId13" sheetId="11"/>
+    <sheet name="chrome_Results_20250903_100726" r:id="rId14" sheetId="12"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="61">
   <si>
     <t>Language</t>
   </si>
@@ -193,7 +193,7 @@
     <t>title : Introduction to Front-End Development</t>
   </si>
   <si>
-    <t>title : Introduction to Web Development</t>
+    <t>title : HTML, CSS, and Javascript for Web Developers</t>
   </si>
   <si>
     <t>rating : 4.8</t>
@@ -203,6 +203,9 @@
   </si>
   <si>
     <t>duration : 1 - 4 Weeks</t>
+  </si>
+  <si>
+    <t>duration : 1 - 3 Months</t>
   </si>
 </sst>
 </file>
@@ -1123,7 +1126,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B48"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1131,34 +1134,257 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="12">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s" s="12">
-        <v>54</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>56</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>57</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>58</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>59</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>59</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="0">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="0">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="0">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="0">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="0">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="0">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="0">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="0">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="0">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s" s="0">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s" s="0">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s" s="0">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s" s="0">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s" s="0">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="0">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s" s="0">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s" s="0">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s" s="0">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s" s="0">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s" s="0">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s" s="0">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="0">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="0">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="0">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="0">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="0">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1436,7 +1662,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B48"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1444,257 +1670,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="3">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s" s="3">
-        <v>1</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>2</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>3</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>5</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>6</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s" s="0">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s" s="0">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s" s="0">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s" s="0">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s" s="0">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s" s="0">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s" s="0">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s" s="0">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s" s="0">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s" s="0">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s" s="0">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s" s="0">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s" s="0">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s" s="0">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s" s="0">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s" s="0">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s" s="0">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s" s="0">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s" s="0">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s" s="0">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="s" s="0">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="s" s="0">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="s" s="0">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="s" s="0">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="s" s="0">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="s" s="0">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="s" s="0">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="s" s="0">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="s" s="0">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="s" s="0">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="s" s="0">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="s" s="0">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="s" s="0">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="s" s="0">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="s" s="0">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="s" s="0">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="s" s="0">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="s" s="0">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="s" s="0">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="s" s="0">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="s" s="0">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="s" s="0">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="s" s="0">
-        <v>52</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1704,7 +1707,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B48"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1712,257 +1715,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="4">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s" s="4">
-        <v>0</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>2</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>3</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>5</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>6</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s" s="0">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s" s="0">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s" s="0">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s" s="0">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s" s="0">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s" s="0">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s" s="0">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s" s="0">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s" s="0">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s" s="0">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s" s="0">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s" s="0">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s" s="0">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s" s="0">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s" s="0">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s" s="0">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s" s="0">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s" s="0">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s" s="0">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s" s="0">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="s" s="0">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="s" s="0">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="s" s="0">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="s" s="0">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="s" s="0">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="s" s="0">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="s" s="0">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="s" s="0">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="s" s="0">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="s" s="0">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="s" s="0">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="s" s="0">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="s" s="0">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="s" s="0">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="s" s="0">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="s" s="0">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="s" s="0">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="s" s="0">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="s" s="0">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="s" s="0">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="s" s="0">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="s" s="0">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="s" s="0">
-        <v>52</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1983,7 +1763,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2">
@@ -2251,7 +2031,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2">
@@ -2508,7 +2288,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B48"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2516,257 +2296,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="7">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s" s="7">
-        <v>0</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>2</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>3</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>5</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>6</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s" s="0">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s" s="0">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s" s="0">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s" s="0">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s" s="0">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s" s="0">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s" s="0">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s" s="0">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s" s="0">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s" s="0">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s" s="0">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s" s="0">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s" s="0">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s" s="0">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s" s="0">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s" s="0">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s" s="0">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s" s="0">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s" s="0">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s" s="0">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="s" s="0">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="s" s="0">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="s" s="0">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="s" s="0">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="s" s="0">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="s" s="0">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="s" s="0">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="s" s="0">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="s" s="0">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="s" s="0">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="s" s="0">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="s" s="0">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="s" s="0">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="s" s="0">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="s" s="0">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="s" s="0">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="s" s="0">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="s" s="0">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="s" s="0">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="s" s="0">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="s" s="0">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="s" s="0">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="s" s="0">
-        <v>52</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -2776,7 +2333,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B48"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2784,257 +2341,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="8">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s" s="8">
-        <v>0</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>2</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>3</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>5</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>6</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s" s="0">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s" s="0">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s" s="0">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s" s="0">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s" s="0">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s" s="0">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s" s="0">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s" s="0">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s" s="0">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s" s="0">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s" s="0">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s" s="0">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s" s="0">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s" s="0">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s" s="0">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s" s="0">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s" s="0">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s" s="0">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s" s="0">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s" s="0">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="s" s="0">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="s" s="0">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="s" s="0">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="s" s="0">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="s" s="0">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="s" s="0">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="s" s="0">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="s" s="0">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="s" s="0">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="s" s="0">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="s" s="0">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="s" s="0">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="s" s="0">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="s" s="0">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="s" s="0">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="s" s="0">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="s" s="0">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="s" s="0">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="s" s="0">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="s" s="0">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="s" s="0">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="s" s="0">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="s" s="0">
-        <v>52</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -3055,7 +2389,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2">

</xml_diff>